<commit_message>
Fixed when there are errors on the Legal Reporting page to refresh the Property listing
</commit_message>
<xml_diff>
--- a/LW_Web/_Templates/_Template - Tenant_Arrears.xlsx
+++ b/LW_Web/_Templates/_Template - Tenant_Arrears.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Source\Repos\lemlewolff\LW_Web\_Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1F9AE0-3840-4572-84C6-30534ADAFBA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F9FF7A-B910-4C99-BB00-48B71E7F663B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="555" windowWidth="25980" windowHeight="15045" tabRatio="212" xr2:uid="{6455282C-9733-4B18-88B6-55E0A49963C2}"/>
+    <workbookView xWindow="1155" yWindow="570" windowWidth="27255" windowHeight="14655" tabRatio="212" xr2:uid="{6455282C-9733-4B18-88B6-55E0A49963C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="57">
   <si>
     <t>Legend</t>
   </si>
@@ -195,13 +195,25 @@
   </si>
   <si>
     <t>Lease End Date</t>
+  </si>
+  <si>
+    <t>Expired Lease</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>Last Note &gt; 45 Days</t>
+  </si>
+  <si>
+    <t>KEY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,8 +252,24 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFA80000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -272,8 +300,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD5D5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF006080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -434,42 +474,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -483,9 +526,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -530,6 +570,34 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -548,15 +616,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -580,13 +639,51 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFD5D5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFA80000"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF006080"/>
+      <color rgb="FFA80000"/>
+      <color rgb="FFFFD5D5"/>
+      <color rgb="FF69472D"/>
+      <color rgb="FFC09200"/>
+      <color rgb="FFFFC1C1"/>
+      <color rgb="FFFFCDC1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -916,10 +1013,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D3D621A-9594-4DC5-BEAB-55FA428C4FC8}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Q12"/>
+  <dimension ref="A1:Q13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:B11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -929,403 +1026,421 @@
     <col min="4" max="4" width="11.7109375" customWidth="1"/>
     <col min="5" max="5" width="37.140625" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" style="26" customWidth="1"/>
-    <col min="8" max="8" width="19.5703125" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="26" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" style="21" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" style="26" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="21" customWidth="1"/>
     <col min="10" max="10" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="26"/>
-    <col min="12" max="12" width="8.140625" style="26" customWidth="1"/>
-    <col min="13" max="13" width="9.85546875" style="26" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="21"/>
+    <col min="12" max="12" width="8.140625" style="21" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" style="21" customWidth="1"/>
     <col min="14" max="14" width="22.85546875" customWidth="1"/>
     <col min="15" max="15" width="12.42578125" customWidth="1"/>
     <col min="16" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41" t="s">
+      <c r="A1" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41" t="s">
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="41"/>
-      <c r="J1" s="41"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="8"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43" t="s">
+      <c r="B2" s="45"/>
+      <c r="C2" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="44"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="46"/>
+      <c r="E2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="32" t="s">
+      <c r="K2" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="8"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="50"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="45" t="s">
+      <c r="A3" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46" t="s">
+      <c r="B3" s="48"/>
+      <c r="C3" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="47"/>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="6">
-        <f>COUNTIFS(F13:F1000000, "&lt;=5000")</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="13">
-        <f>SUMIFS(F13:F1000000, F13:F1000000, "&lt;=5000")</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="5" t="s">
+      <c r="F3" s="4">
+        <f>COUNTIFS(F13:F999227, "&lt;=5000")</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <f>SUMIFS(F13:F999227, F13:F999227, "&lt;=5000")</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="6">
-        <f>COUNTIFS(K13:K1000000, "LKEM", G13:G1000000, "&lt;&gt;")</f>
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <f>COUNTIFS(K13:K1000000, "Horing", G13:G1000000, "&lt;&gt;")</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="32"/>
-      <c r="L3" s="27"/>
+      <c r="I3" s="4">
+        <f>COUNTIFS(K13:K999227, "LKEM", G13:G999227, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="4">
+        <f>COUNTIFS(K13:K999227, "Horing", G13:G999227, "&lt;&gt;")</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="37"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="51"/>
+      <c r="N3" s="52" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35" t="s">
+      <c r="B4" s="40"/>
+      <c r="C4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="8" t="s">
+      <c r="D4" s="41"/>
+      <c r="E4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8">
-        <f>COUNTIFS(F13:F1000000, "&gt;5000", F13:F1000000, "&lt;=10000")</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="9">
-        <f ca="1">SUMIFS(F13:F1000000, F13:F1000000, "&gt;5000", F13:F1000000, "&lt;=10000")</f>
-        <v>0</v>
-      </c>
-      <c r="H4" s="7" t="s">
+      <c r="F4" s="5">
+        <f>COUNTIFS(F13:F999227, "&gt;5000", F13:F999227, "&lt;=10000")</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="6">
+        <f>SUMIFS(F13:F999227, F13:F999227, "&gt;5000", F13:F999227, "&lt;=10000")</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="I4" s="8">
-        <f>COUNTIFS(K13:K1000000, "LKEM", I13:I1000000, "&gt;30")</f>
-        <v>0</v>
-      </c>
-      <c r="J4" s="8">
-        <f>COUNTIFS(K13:K1000000, "horing", I13:I1000000, "&gt;30")</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="32"/>
-      <c r="L4" s="28"/>
+      <c r="I4" s="5">
+        <f>COUNTIFS(K13:K999227, "LKEM", I13:I999227, "&gt;30")</f>
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <f>COUNTIFS(K13:K999227, "horing", I13:I999227, "&gt;30")</f>
+        <v>0</v>
+      </c>
+      <c r="K4" s="37"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="53" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" s="52" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="33" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38" t="s">
+      <c r="B5" s="34"/>
+      <c r="C5" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="39"/>
-      <c r="E5" s="11" t="s">
+      <c r="D5" s="35"/>
+      <c r="E5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="11">
-        <f>COUNTIFS(F13:F1000000, "&gt;10000", F13:F1000000, "&lt;=20000")</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="13">
-        <f ca="1">SUMIFS(F13:F1000000, F13:F1000000, "&gt;10000", F13:F1000000, "&lt;=20000")</f>
-        <v>0</v>
-      </c>
-      <c r="H5" s="10" t="s">
+      <c r="F5" s="7">
+        <f>COUNTIFS(F13:F999227, "&gt;10000", F13:F999227, "&lt;=20000")</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <f>SUMIFS(F13:F999227, F13:F999227, "&gt;10000", F13:F999227, "&lt;=20000")</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="6">
-        <f>COUNTIFS(K13:K1000000, "LKEM", G13:G1000000, "Closed")</f>
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <f>COUNTIFS(K13:K1000000, "Horing", G13:G1000000, "closed")</f>
-        <v>0</v>
-      </c>
-      <c r="K5" s="32"/>
-      <c r="L5" s="28"/>
+      <c r="I5" s="4">
+        <f>COUNTIFS(K13:K999227, "LKEM", G13:G999227, "Closed")</f>
+        <v>0</v>
+      </c>
+      <c r="J5" s="4">
+        <f>COUNTIFS(K13:K999227, "Horing", G13:G999227, "closed")</f>
+        <v>0</v>
+      </c>
+      <c r="K5" s="37"/>
+      <c r="L5" s="23"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35" t="s">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="36"/>
-      <c r="E6" s="8" t="s">
+      <c r="D6" s="41"/>
+      <c r="E6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="8">
-        <f>COUNTIFS(F13:F1000000, "&gt;20000", F13:F1000000, "&lt;=30000")</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="9">
-        <f ca="1">SUMIFS(F13:F1000000, F13:F1000000, "&gt;20000", F13:F1000000, "&lt;=30000")</f>
-        <v>0</v>
-      </c>
-      <c r="H6" s="7"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="32"/>
-      <c r="L6" s="28"/>
+      <c r="F6" s="5">
+        <f>COUNTIFS(F13:F999227, "&gt;20000", F13:F999227, "&lt;=30000")</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="6">
+        <f>SUMIFS(F13:F999227, F13:F999227, "&gt;20000", F13:F999227, "&lt;=30000")</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="29"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="23"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="34" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="39"/>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="35"/>
+      <c r="E7" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="14">
-        <f>COUNTIFS(F13:F1000000, "&gt;30000", F13:F1000000, "&lt;=40000")</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="15">
-        <f ca="1">SUMIFS(F13:F1000000, F13:F1000000, "&gt;30000", F13:F1000000, "&lt;=40000")</f>
-        <v>0</v>
-      </c>
-      <c r="H7" s="16" t="s">
+      <c r="F7" s="10">
+        <f>COUNTIFS(F13:F999227, "&gt;30000", F13:F999227, "&lt;=40000")</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="11">
+        <f>SUMIFS(F13:F999227, F13:F999227, "&gt;30000", F13:F999227, "&lt;=40000")</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="I7" s="17">
+      <c r="I7" s="12">
         <f>I3-I4</f>
         <v>0</v>
       </c>
-      <c r="J7" s="17">
+      <c r="J7" s="12">
         <f>J3-J4</f>
         <v>0</v>
       </c>
-      <c r="K7" s="31" t="s">
+      <c r="K7" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="L7" s="28"/>
+      <c r="L7" s="23"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="34" t="s">
+      <c r="A8" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35" t="s">
+      <c r="B8" s="40"/>
+      <c r="C8" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="8" t="s">
+      <c r="D8" s="41"/>
+      <c r="E8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="8">
-        <f>COUNTIFS(F13:F1000000, "&gt;40000", F13:F1000000, "&lt;=50000")</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="18">
-        <f ca="1">SUMIFS(F13:F1000000, F13:F1000000, "&gt;40000", F13:F1000000, "&lt;=50000")</f>
-        <v>0</v>
-      </c>
-      <c r="H8" s="7" t="s">
+      <c r="F8" s="5">
+        <f>COUNTIFS(F13:F999227, "&gt;40000", F13:F999227, "&lt;=50000")</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="13">
+        <f>SUMIFS(F13:F999227, F13:F999227, "&gt;40000", F13:F999227, "&lt;=50000")</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="I8" s="19" t="e">
+      <c r="I8" s="14" t="e">
         <f>ROUND(I7/I3, 2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="J8" s="19" t="e">
+      <c r="J8" s="14" t="e">
         <f>ROUND(J7/J3, 2)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="32"/>
-      <c r="L8" s="8"/>
+      <c r="K8" s="37"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="37"/>
-      <c r="B9" s="38"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="11" t="s">
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="11">
-        <f>COUNTIFS(F13:F1000000, "&gt;50000", F13:F1000000, "&lt;100000")</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="13">
-        <f ca="1">SUMIFS(F13:F1000000, F13:F1000000, "&gt;50000", F13:F1000000, "&lt;100000")</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="32"/>
-      <c r="L9" s="8"/>
+      <c r="F9" s="7">
+        <f>COUNTIFS(F13:F999227, "&gt;50000", F13:F999227, "&lt;100000")</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <f>SUMIFS(F13:F999227, F13:F999227, "&gt;50000", F13:F999227, "&lt;100000")</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="5"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="8" t="s">
+      <c r="A10" s="39"/>
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="8">
-        <f>COUNTIFS(F13:F1000000, "&gt;=100000")</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="9">
-        <f>SUMIFS(F13:F1000000, F13:F1000000, "&gt;=100000")</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="7"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="32"/>
-      <c r="L10" s="8"/>
+      <c r="F10" s="5">
+        <f>COUNTIFS(F13:F999227, "&gt;=100000")</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="6">
+        <f>SUMIFS(F13:F999227, F13:F999227, "&gt;=100000")</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="29"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="37"/>
+      <c r="L10" s="5"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="37"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="20" t="s">
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="16">
         <f>SUM(F3:F10)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="22">
-        <f ca="1">SUM(G3:G10)</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="8"/>
+      <c r="G11" s="17">
+        <f>SUM(G3:G10)</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="30"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:17" ht="30" customHeight="1">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="F12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="J12" s="25" t="s">
+      <c r="J12" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="L12" s="30" t="s">
+      <c r="L12" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="M12" s="30" t="s">
+      <c r="M12" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="N12" s="30" t="s">
+      <c r="N12" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="O12" s="30" t="s">
+      <c r="O12" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="P12" s="30" t="s">
+      <c r="P12" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="Q12" s="30" t="s">
+      <c r="Q12" s="25" t="s">
         <v>52</v>
       </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="Q13" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="24">
+  <mergeCells count="25">
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="K2:K6"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="C4:D4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="C6:D6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="K7:K11"/>
@@ -1337,6 +1452,14 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C11:D11"/>
   </mergeCells>
+  <conditionalFormatting sqref="A13:Q9227">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>AND($I13&lt;&gt;"",$I13&gt;45)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="2">
+      <formula>AND($Q13&lt;TODAY(),$B13&lt;&gt;"")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>